<commit_message>
Changes to graphs, added lab font
</commit_message>
<xml_diff>
--- a/Data/Vacancy Rates Comparison.xlsx
+++ b/Data/Vacancy Rates Comparison.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ah6535\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbc9285\Documents\GitHub\hsl-vacancy-rates\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,6 @@
     <sheet name="5-year" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -24,9 +23,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="9">
   <si>
     <t>Span</t>
-  </si>
-  <si>
-    <t>Year(s)</t>
   </si>
   <si>
     <t>Rate</t>
@@ -48,6 +44,9 @@
   </si>
   <si>
     <t>5-year</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -309,35 +308,44 @@
                 <c:f>'1-year'!$D$1:$D$13</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="10"/>
+                  <c:ptCount val="13"/>
                   <c:pt idx="0">
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>3.5999999999999997E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
                     <c:v>0.03</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="3">
+                    <c:v>0.03</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
                     <c:v>2.4E-2</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="5">
                     <c:v>0.04</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="6">
                     <c:v>4.7E-2</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="7">
                     <c:v>4.1000000000000002E-2</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="8">
                     <c:v>3.5999999999999997E-2</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="9">
                     <c:v>3.7999999999999999E-2</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="10">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
                     <c:v>4.7E-2</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="12">
                     <c:v>2.3E-2</c:v>
                   </c:pt>
                 </c:numCache>
@@ -348,35 +356,44 @@
                 <c:f>'1-year'!$D$1:$D$13</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="10"/>
+                  <c:ptCount val="13"/>
                   <c:pt idx="0">
                     <c:v>0</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>3.5999999999999997E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
                     <c:v>0.03</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="3">
+                    <c:v>0.03</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
                     <c:v>2.4E-2</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="5">
                     <c:v>0.04</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="6">
                     <c:v>4.7E-2</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="7">
                     <c:v>4.1000000000000002E-2</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="8">
                     <c:v>3.5999999999999997E-2</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="9">
                     <c:v>3.7999999999999999E-2</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="10">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
                     <c:v>4.7E-2</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="12">
                     <c:v>2.3E-2</c:v>
                   </c:pt>
                 </c:numCache>
@@ -406,32 +423,41 @@
                 <c:f>'1-year'!$D$2:$D$13</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="9"/>
+                  <c:ptCount val="12"/>
                   <c:pt idx="0">
+                    <c:v>3.5999999999999997E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
                     <c:v>0.03</c:v>
                   </c:pt>
-                  <c:pt idx="1">
+                  <c:pt idx="2">
+                    <c:v>0.03</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
                     <c:v>2.4E-2</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="4">
                     <c:v>0.04</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="5">
                     <c:v>4.7E-2</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="6">
                     <c:v>4.1000000000000002E-2</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="7">
                     <c:v>3.5999999999999997E-2</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="8">
                     <c:v>3.7999999999999999E-2</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="9">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>4.7E-2</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="11">
                     <c:v>2.3E-2</c:v>
                   </c:pt>
                 </c:numCache>
@@ -442,32 +468,41 @@
                 <c:f>'1-year'!$D$2:$D$13</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="9"/>
+                  <c:ptCount val="12"/>
                   <c:pt idx="0">
+                    <c:v>3.5999999999999997E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
                     <c:v>0.03</c:v>
                   </c:pt>
-                  <c:pt idx="1">
+                  <c:pt idx="2">
+                    <c:v>0.03</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
                     <c:v>2.4E-2</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="4">
                     <c:v>0.04</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="5">
                     <c:v>4.7E-2</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="6">
                     <c:v>4.1000000000000002E-2</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="7">
                     <c:v>3.5999999999999997E-2</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="8">
                     <c:v>3.7999999999999999E-2</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="9">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
                     <c:v>4.7E-2</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="11">
                     <c:v>2.3E-2</c:v>
                   </c:pt>
                 </c:numCache>
@@ -492,32 +527,41 @@
               <c:f>'1-year'!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>2013</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>2014</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>2015</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>2016</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>2017</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>2018</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>2019</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>2021</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>2022</c:v>
                 </c:pt>
               </c:numCache>
@@ -528,32 +572,41 @@
               <c:f>'1-year'!$C$2:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>5.0999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>3.9E-2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>0.05</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="4">
                   <c:v>0.106</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>0.105</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>0.1</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>8.3000000000000004E-2</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
                   <c:v>9.6000000000000002E-2</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.108</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>3.4000000000000002E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -803,6 +856,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2501,7 +2555,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2511,24 +2565,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="14.25">
+      <c r="A2" s="6" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="14.25" hidden="1">
-      <c r="A2" s="6" t="s">
-        <v>6</v>
       </c>
       <c r="B2" s="6">
         <v>2011</v>
@@ -2548,9 +2602,9 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.25" hidden="1">
+    <row r="3" spans="1:6" ht="14.25">
       <c r="A3" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="6">
         <v>2012</v>
@@ -2572,7 +2626,7 @@
     </row>
     <row r="4" spans="1:6" ht="14.25">
       <c r="A4" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="6">
         <v>2013</v>
@@ -2594,7 +2648,7 @@
     </row>
     <row r="5" spans="1:6" ht="14.25">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3">
         <v>2014</v>
@@ -2616,7 +2670,7 @@
     </row>
     <row r="6" spans="1:6" ht="14.25">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3">
         <v>2015</v>
@@ -2638,7 +2692,7 @@
     </row>
     <row r="7" spans="1:6" ht="14.25">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="3">
         <v>2016</v>
@@ -2660,7 +2714,7 @@
     </row>
     <row r="8" spans="1:6" ht="14.25">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3">
         <v>2017</v>
@@ -2682,7 +2736,7 @@
     </row>
     <row r="9" spans="1:6" ht="14.25">
       <c r="A9" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="3">
         <v>2018</v>
@@ -2704,7 +2758,7 @@
     </row>
     <row r="10" spans="1:6" ht="14.25">
       <c r="A10" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="3">
         <v>2019</v>
@@ -2724,18 +2778,18 @@
         <v>0.13400000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.25" hidden="1">
+    <row r="11" spans="1:6" ht="14.25">
       <c r="A11" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="3">
         <v>2020</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" s="7" t="e">
         <f t="shared" si="0"/>
@@ -2748,7 +2802,7 @@
     </row>
     <row r="12" spans="1:6" ht="14.25">
       <c r="A12" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="3">
         <v>2021</v>
@@ -2770,7 +2824,7 @@
     </row>
     <row r="13" spans="1:6" ht="14.25">
       <c r="A13" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="3">
         <v>2022</v>
@@ -2804,8 +2858,8 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2815,24 +2869,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="14.25" hidden="1">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3">
         <v>2014</v>
@@ -2854,7 +2908,7 @@
     </row>
     <row r="3" spans="1:6" ht="14.25" hidden="1">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3">
         <v>2015</v>
@@ -2876,7 +2930,7 @@
     </row>
     <row r="4" spans="1:6" ht="14.25" hidden="1">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3">
         <v>2016</v>
@@ -2898,7 +2952,7 @@
     </row>
     <row r="5" spans="1:6" ht="14.25">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3">
         <v>2017</v>
@@ -2920,7 +2974,7 @@
     </row>
     <row r="6" spans="1:6" ht="14.25" hidden="1">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3">
         <v>2018</v>
@@ -2942,7 +2996,7 @@
     </row>
     <row r="7" spans="1:6" ht="14.25" hidden="1" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3">
         <v>2019</v>
@@ -2964,7 +3018,7 @@
     </row>
     <row r="8" spans="1:6" ht="14.25" hidden="1" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3">
         <v>2020</v>
@@ -2986,7 +3040,7 @@
     </row>
     <row r="9" spans="1:6" ht="14.25" hidden="1">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3">
         <v>2021</v>
@@ -3008,7 +3062,7 @@
     </row>
     <row r="10" spans="1:6" ht="14.25">
       <c r="A10" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="3">
         <v>2022</v>

</xml_diff>